<commit_message>
Add capability to generate form by student ID
</commit_message>
<xml_diff>
--- a/examples/students_groups.xlsx
+++ b/examples/students_groups.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chat/local_git/webpa-offline/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chat/local_git/webpa-offline/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75CD03C-7BF4-FD4D-B2CA-A1CB37F3851E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36C6A81-50D5-124C-8B00-CD3EA3E0BA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="2520" windowWidth="20620" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Person</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Elaine</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -917,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -929,132 +932,180 @@
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>100001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>100002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>100003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>100004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>100005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>100006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>100007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>100008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>100009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>100010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>100011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>100012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>100013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>100014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16">
         <v>3</v>
+      </c>
+      <c r="C16">
+        <v>100015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>